<commit_message>
yorum ve bug düzeltme
</commit_message>
<xml_diff>
--- a/data/lessons/BLM001/table1.xlsx
+++ b/data/lessons/BLM001/table1.xlsx
@@ -616,7 +616,7 @@
         <v>1</v>
       </c>
       <c r="G8" t="n">
-        <v>0.2200231481481482</v>
+        <v>0.2200038580246914</v>
       </c>
     </row>
     <row r="9">
@@ -639,7 +639,7 @@
         <v>1</v>
       </c>
       <c r="G9" t="n">
-        <v>0.2200231481481482</v>
+        <v>0.2200038580246914</v>
       </c>
     </row>
     <row r="10">
@@ -662,7 +662,7 @@
         <v>1</v>
       </c>
       <c r="G10" t="n">
-        <v>0.7400077160493828</v>
+        <v>0.7400012860082305</v>
       </c>
     </row>
     <row r="11">
@@ -708,7 +708,7 @@
         <v>0</v>
       </c>
       <c r="G12" t="n">
-        <v>0.4600180041152263</v>
+        <v>0.460003000685871</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
dizin ve branch düzenlemesi
</commit_message>
<xml_diff>
--- a/data/lessons/BLM001/table1.xlsx
+++ b/data/lessons/BLM001/table1.xlsx
@@ -616,7 +616,7 @@
         <v>1</v>
       </c>
       <c r="G8" t="n">
-        <v>0.2200038580246914</v>
+        <v>0.2200000000000001</v>
       </c>
     </row>
     <row r="9">
@@ -639,7 +639,7 @@
         <v>1</v>
       </c>
       <c r="G9" t="n">
-        <v>0.2200038580246914</v>
+        <v>0.2200000000000001</v>
       </c>
     </row>
     <row r="10">
@@ -662,7 +662,7 @@
         <v>1</v>
       </c>
       <c r="G10" t="n">
-        <v>0.7400012860082305</v>
+        <v>0.7400000000000001</v>
       </c>
     </row>
     <row r="11">
@@ -708,7 +708,7 @@
         <v>0</v>
       </c>
       <c r="G12" t="n">
-        <v>0.460003000685871</v>
+        <v>0.46</v>
       </c>
     </row>
   </sheetData>

</xml_diff>